<commit_message>
update the coding from Stahl lab after they sent a correction
</commit_message>
<xml_diff>
--- a/data/after coding/data_awareness_for_hand_scoring_Stahl_integrated.xlsx
+++ b/data/after coding/data_awareness_for_hand_scoring_Stahl_integrated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmoranyo\Documents\GitHub\unconscious-ec-RRR\data\after coding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1CA9149-6CBD-492A-8A52-64C9F59AA447}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{35424FBA-9824-4B39-ADF3-E2B975ADC14A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2776" uniqueCount="314">
   <si>
     <t>unique_id</t>
   </si>
@@ -956,6 +956,12 @@
   </si>
   <si>
     <t>TRUE</t>
+  </si>
+  <si>
+    <t>fazio_and_olsen_criteria_consense</t>
+  </si>
+  <si>
+    <t>fazio_and_olsen_modified_criteria_consense</t>
   </si>
 </sst>
 </file>
@@ -997,9 +1003,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1282,18 +1289,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="F102" sqref="F102"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.7265625" customWidth="1"/>
     <col min="2" max="3" width="16.1796875" customWidth="1"/>
-    <col min="5" max="5" width="8.6328125" customWidth="1"/>
-    <col min="6" max="6" width="9.6328125" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" customWidth="1"/>
-    <col min="8" max="8" width="9.7265625" customWidth="1"/>
+    <col min="5" max="5" width="32.7265625" customWidth="1"/>
+    <col min="6" max="6" width="41.1796875" customWidth="1"/>
+    <col min="7" max="7" width="32.453125" customWidth="1"/>
+    <col min="8" max="8" width="40.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -1650,14 +1657,14 @@
       <c r="E14" t="s">
         <v>310</v>
       </c>
-      <c r="F14" t="s">
-        <v>311</v>
+      <c r="F14" s="2" t="s">
+        <v>310</v>
       </c>
       <c r="G14" t="s">
         <v>310</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>